<commit_message>
Created publisher only from excel data
</commit_message>
<xml_diff>
--- a/exo_control/neural_network_parameters/excel/PV_cp_cnn.xlsx
+++ b/exo_control/neural_network_parameters/excel/PV_cp_cnn.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,204 +483,1322 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.3928256332874298</v>
+        <v>5.653803825378418</v>
       </c>
       <c r="D2" t="n">
-        <v>-9.352646827697754</v>
+        <v>-9.45506477355957</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.6886233687400818</v>
+        <v>-4.90446662902832</v>
       </c>
       <c r="F2" t="n">
-        <v>-15.5637674331665</v>
+        <v>-9.836400032043457</v>
       </c>
       <c r="G2" t="n">
-        <v>-4.695226669311523</v>
+        <v>-1.899656057357788</v>
       </c>
       <c r="H2" t="n">
-        <v>1.087006330490112</v>
+        <v>0.6799779534339905</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-2.591481070518494</v>
+        <v>-0.03955951504409314</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0447062923014164</v>
+        <v>0.1568202170729637</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.3333061635494232</v>
+        <v>6.982532501220703</v>
       </c>
       <c r="D3" t="n">
-        <v>-9.565400123596191</v>
+        <v>-7.362154483795166</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.6755387783050537</v>
+        <v>-5.915628433227539</v>
       </c>
       <c r="F3" t="n">
-        <v>-15.49340343475342</v>
+        <v>-10.17363929748535</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.417865753173828</v>
+        <v>0.1271894425153732</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9270286560058594</v>
+        <v>-3.742504596710205</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-7.136664896011353</v>
+        <v>0.0760839606821537</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.03403839081525803</v>
+        <v>-0.7650198936462402</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.2289153039455414</v>
+        <v>3.098288774490356</v>
       </c>
       <c r="D4" t="n">
-        <v>-9.467032432556152</v>
+        <v>-7.170287609100342</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.55617755651474</v>
+        <v>-5.422814846038818</v>
       </c>
       <c r="F4" t="n">
-        <v>-15.51019382476807</v>
+        <v>-8.191237449645996</v>
       </c>
       <c r="G4" t="n">
-        <v>-4.708047866821289</v>
+        <v>3.839830875396729</v>
       </c>
       <c r="H4" t="n">
-        <v>1.027120471000671</v>
+        <v>-8.351227760314941</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.53</v>
+        <v>0.07078120946884156</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1073158232867718</v>
+        <v>-1.576290118694305</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.4049983322620392</v>
+        <v>3.276397943496704</v>
       </c>
       <c r="D5" t="n">
-        <v>-9.753512382507324</v>
+        <v>-4.016393184661865</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.6086620092391968</v>
+        <v>-5.721666812896729</v>
       </c>
       <c r="F5" t="n">
-        <v>-15.39486122131348</v>
+        <v>-6.446614265441895</v>
       </c>
       <c r="G5" t="n">
-        <v>-4.490975379943848</v>
+        <v>6.625461578369141</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9756739139556885</v>
+        <v>-8.255023956298828</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-2.29799102306366</v>
+        <v>0.149731317460537</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1404495659470558</v>
+        <v>-1.888343858718872</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3400468528270721</v>
+        <v>0.6246141791343689</v>
       </c>
       <c r="D6" t="n">
-        <v>-10.00685214996338</v>
+        <v>-2.865157127380371</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.8244520425796509</v>
+        <v>-4.726386070251465</v>
       </c>
       <c r="F6" t="n">
-        <v>-15.78482341766357</v>
+        <v>-5.775547981262207</v>
       </c>
       <c r="G6" t="n">
-        <v>-4.971243381500244</v>
+        <v>12.28879928588867</v>
       </c>
       <c r="H6" t="n">
-        <v>1.091367602348328</v>
+        <v>-9.456803321838379</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-7.334595060348511</v>
+        <v>0.1488613161444664</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1707112380862236</v>
+        <v>-0.7408175563812256</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.2243693768978119</v>
+        <v>0.6538363099098206</v>
       </c>
       <c r="D7" t="n">
-        <v>-10.36881256103516</v>
+        <v>-7.128524303436279</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.8310400247573853</v>
+        <v>-5.34001350402832</v>
       </c>
       <c r="F7" t="n">
-        <v>-15.83245277404785</v>
+        <v>-8.243284225463867</v>
       </c>
       <c r="G7" t="n">
-        <v>-4.71468448638916</v>
+        <v>11.89204502105713</v>
       </c>
       <c r="H7" t="n">
-        <v>1.072893142700195</v>
+        <v>-10.34447765350342</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-27.24758094787598</v>
+        <v>0.08749550953507423</v>
       </c>
       <c r="B8" t="n">
-        <v>0.4154803431034088</v>
+        <v>-3.7135080575943</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2329792678356171</v>
+        <v>2.714996576309204</v>
       </c>
       <c r="D8" t="n">
-        <v>-10.31872272491455</v>
+        <v>-4.651477813720703</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.117427229881287</v>
+        <v>-3.041460037231445</v>
       </c>
       <c r="F8" t="n">
-        <v>-16.21769905090332</v>
+        <v>-1.850562691688538</v>
       </c>
       <c r="G8" t="n">
-        <v>-5.112422466278076</v>
+        <v>10.56995105743408</v>
       </c>
       <c r="H8" t="n">
-        <v>1.220522284507751</v>
+        <v>-11.51589393615723</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-27.93366107940674</v>
+        <v>0.1338613751530647</v>
       </c>
       <c r="B9" t="n">
+        <v>-4.032371563911438</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.157655715942383</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-8.476902008056641</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.8703367710113525</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1.164852261543274</v>
+      </c>
+      <c r="G9" t="n">
+        <v>17.68305778503418</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-6.705341815948486</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.2425306838750839</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-4.553830766677857</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.492339611053467</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-6.409841060638428</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.015111923217773</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.04346291720867157</v>
+      </c>
+      <c r="G10" t="n">
+        <v>13.41067504882812</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-4.840447425842285</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.244720171391964</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-4.495678539276123</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-2.565879583358765</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-6.289535999298096</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.3835521340370178</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.1685182899236679</v>
+      </c>
+      <c r="G11" t="n">
+        <v>16.39345359802246</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-1.915578365325928</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.3026859045028686</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-6.227140626907349</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-4.512838363647461</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-6.855685710906982</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.22714900970459</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3.554962158203125</v>
+      </c>
+      <c r="G12" t="n">
+        <v>16.55867767333984</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-2.643069744110107</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.2357800707221031</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-7.360333452224732</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-2.265599489212036</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-2.806259632110596</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.1785293221473694</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5.991874694824219</v>
+      </c>
+      <c r="G13" t="n">
+        <v>15.9516134262085</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.183537840843201</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.3643946492671967</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-7.376822662353516</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-6.585517406463623</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-5.782844543457031</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.989960670471191</v>
+      </c>
+      <c r="F14" t="n">
+        <v>6.027334213256836</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12.59235954284668</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.04213961586356163</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.3006063675880432</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-7.597548503875733</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-4.442989826202393</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-4.515466213226318</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4.235147476196289</v>
+      </c>
+      <c r="F15" t="n">
+        <v>6.502001285552979</v>
+      </c>
+      <c r="G15" t="n">
+        <v>12.2869758605957</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.773665726184845</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.3208064460754395</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-6.547559900283813</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-5.121472358703613</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-7.078282833099365</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5.727447509765625</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4.2440185546875</v>
+      </c>
+      <c r="G16" t="n">
+        <v>6.770132541656494</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2.436364650726318</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.3284795796871186</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-7.392401561737061</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-5.379199504852295</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-4.869113445281982</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5.340146541595459</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.060836791992188</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5.522574424743652</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8118055462837219</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.3895710784196854</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-7.376628570556641</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-7.431145191192627</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-4.544234275817871</v>
+      </c>
+      <c r="E18" t="n">
+        <v>5.811061382293701</v>
+      </c>
+      <c r="F18" t="n">
+        <v>6.026916980743408</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.159028649330139</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2.008039474487305</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.345938048362732</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-7.189318361282349</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-5.965595245361328</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-5.017333507537842</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7.390029907226562</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5.624109745025635</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2.51450514793396</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.768268227577209</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.3840714317560196</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-6.799793815612794</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-7.24642276763916</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-6.374450206756592</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5.963458061218262</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.786443710327148</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-3.265783548355103</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.997541308403015</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.2890308326482773</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-7.633254823684693</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-4.054190158843994</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-7.59557580947876</v>
+      </c>
+      <c r="E21" t="n">
+        <v>7.018465995788574</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6.578786849975586</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-4.501266479492188</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2.374178409576416</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.3386340808868408</v>
+      </c>
+      <c r="B22" t="n">
+        <v>-6.609446372985841</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-5.720269203186035</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-3.579771995544434</v>
+      </c>
+      <c r="E22" t="n">
+        <v>7.549747943878174</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4.377104759216309</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-10.92592334747314</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.854192852973938</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.4411210888624191</v>
+      </c>
+      <c r="B23" t="n">
+        <v>-5.940849161148072</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-9.162611961364746</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-4.251810073852539</v>
+      </c>
+      <c r="E23" t="n">
+        <v>6.078746795654297</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.939297437667847</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-9.47633171081543</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.6368582844734192</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.4456500554084778</v>
+      </c>
+      <c r="B24" t="n">
+        <v>-6.180853271484375</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-9.314731597900391</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-4.079325199127197</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4.485651016235352</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3.455422878265381</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-9.130809783935547</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.1205405294895172</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.491607638001442</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-6.48880467414856</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-10.85835933685303</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-4.731420993804932</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.573874473571777</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4.117667198181152</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-11.33881282806396</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-0.8750782012939453</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.4214950090646744</v>
+      </c>
+      <c r="B26" t="n">
+        <v>-6.662927255630493</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-8.503409385681152</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-2.92297625541687</v>
+      </c>
+      <c r="E26" t="n">
+        <v>4.289812564849854</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4.492114067077637</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-11.95578861236572</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.03409799560904503</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
         <v>0.53</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.248736709356308</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-10.56587314605713</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-1.03658664226532</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-16.3979434967041</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-4.967277526855469</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1.090420961380005</v>
+      <c r="B27" t="n">
+        <v>-6.60126368522644</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-12.14788627624512</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-2.128310680389404</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2.17871880531311</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4.359508037567139</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-11.91915321350098</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-0.1532654166221619</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.4611238217353821</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-7.341657676696777</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-9.834465980529785</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.4804942607879639</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.681118369102478</v>
+      </c>
+      <c r="F28" t="n">
+        <v>5.951713085174561</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-9.12940788269043</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-0.706722617149353</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.3765462678670883</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-6.523819541931153</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-6.993666648864746</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-0.3383738994598389</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-2.455382108688354</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.192965507507324</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-6.344018459320068</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-5.332154750823975</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.3696409088373184</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-7.121702642440797</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-6.76172924041748</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3.226950407028198</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-7.505757331848145</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5.478703498840332</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-7.42233943939209</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-2.978699445724487</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.2783848470449448</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-5.707650899887085</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-3.696612119674683</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.489211082458496</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-8.876958847045898</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2.437807559967041</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-3.759764671325684</v>
+      </c>
+      <c r="H31" t="n">
+        <v>-3.03329873085022</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.3707437318563461</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-6.77438497543335</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-6.798770904541016</v>
+      </c>
+      <c r="D32" t="n">
+        <v>6.546842098236084</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-11.294677734375</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4.731802463531494</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-2.677718639373779</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-4.939930438995361</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.2245207720994949</v>
+      </c>
+      <c r="B33" t="n">
+        <v>-6.712632446289063</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-1.887420892715454</v>
+      </c>
+      <c r="D33" t="n">
+        <v>6.690071105957031</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-11.49570274353027</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.599004745483398</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-5.09229040145874</v>
+      </c>
+      <c r="H33" t="n">
+        <v>-2.373816728591919</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.1530321574211121</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-5.939880723953247</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.5137457251548767</v>
+      </c>
+      <c r="D34" t="n">
+        <v>9.677059173583984</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-12.36382675170898</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2.937215328216553</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-4.109493732452393</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.7524218559265137</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.5760446442309581</v>
+      </c>
+      <c r="B35" t="n">
+        <v>67.12821872158977</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-3.256949663162231</v>
+      </c>
+      <c r="D35" t="n">
+        <v>9.320235252380371</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-12.42622756958008</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.024024367332458</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-2.465534210205078</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.166785255074501</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.9258429132933984</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-598.0477792531145</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2.539982080459595</v>
+      </c>
+      <c r="D36" t="n">
+        <v>12.40510082244873</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-7.936156749725342</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.4885174036026001</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-5.672225475311279</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-1.611362099647522</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.9854273361874343</v>
+      </c>
+      <c r="B37" t="n">
+        <v>6025.956393897622</v>
+      </c>
+      <c r="C37" t="n">
+        <v>2.155580759048462</v>
+      </c>
+      <c r="D37" t="n">
+        <v>12.78581237792969</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-5.631823539733887</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1.626761674880981</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-3.977789640426636</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.4700658321380615</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.9994786432932744</v>
+      </c>
+      <c r="B38" t="n">
+        <v>-49178.69888090814</v>
+      </c>
+      <c r="C38" t="n">
+        <v>5.016924381256104</v>
+      </c>
+      <c r="D38" t="n">
+        <v>12.49951267242432</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.9030991792678833</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-0.5329524874687195</v>
+      </c>
+      <c r="G38" t="n">
+        <v>-1.772716522216797</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.688389897346497</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.9999257146760382</v>
+      </c>
+      <c r="B39" t="n">
+        <v>433650.9197279753</v>
+      </c>
+      <c r="C39" t="n">
+        <v>3.117336511611938</v>
+      </c>
+      <c r="D39" t="n">
+        <v>11.91916275024414</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2.331615924835205</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.2135843187570572</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-3.424475431442261</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1.144328236579895</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.999999749297701</v>
+      </c>
+      <c r="B40" t="n">
+        <v>-3191328.746648094</v>
+      </c>
+      <c r="C40" t="n">
+        <v>5.593725681304932</v>
+      </c>
+      <c r="D40" t="n">
+        <v>11.59312152862549</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.168919086456299</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-1.448671698570251</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-3.680985927581787</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1.698674321174622</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1.000000001762465</v>
+      </c>
+      <c r="B41" t="n">
+        <v>19699683.16564975</v>
+      </c>
+      <c r="C41" t="n">
+        <v>5.778951644897461</v>
+      </c>
+      <c r="D41" t="n">
+        <v>10.50806140899658</v>
+      </c>
+      <c r="E41" t="n">
+        <v>6.034224510192871</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-2.800826549530029</v>
+      </c>
+      <c r="G41" t="n">
+        <v>-4.035259246826172</v>
+      </c>
+      <c r="H41" t="n">
+        <v>3.173066854476929</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.9999999997511972</v>
+      </c>
+      <c r="B42" t="n">
+        <v>-65333767.48886446</v>
+      </c>
+      <c r="C42" t="n">
+        <v>8.166824340820312</v>
+      </c>
+      <c r="D42" t="n">
+        <v>8.219392776489258</v>
+      </c>
+      <c r="E42" t="n">
+        <v>5.934537410736084</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-6.056411743164062</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-9.089858055114746</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3.366066932678223</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.9999999999789329</v>
+      </c>
+      <c r="B43" t="n">
+        <v>327212862.8340886</v>
+      </c>
+      <c r="C43" t="n">
+        <v>4.14646053314209</v>
+      </c>
+      <c r="D43" t="n">
+        <v>5.195571422576904</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.621502876281738</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-4.128128528594971</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-5.493937492370605</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2.301235914230347</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1.000000000001789</v>
+      </c>
+      <c r="B44" t="n">
+        <v>-629447671.9172032</v>
+      </c>
+      <c r="C44" t="n">
+        <v>7.165080070495605</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2.994858026504517</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3.516398429870605</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-7.64389181137085</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-8.68282413482666</v>
+      </c>
+      <c r="H44" t="n">
+        <v>3.219171047210693</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.9999999999998302</v>
+      </c>
+      <c r="B45" t="n">
+        <v>782869358.9793085</v>
+      </c>
+      <c r="C45" t="n">
+        <v>7.343530654907227</v>
+      </c>
+      <c r="D45" t="n">
+        <v>-0.4419060945510864</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4.416713237762451</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-8.418839454650879</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-9.380785942077637</v>
+      </c>
+      <c r="H45" t="n">
+        <v>4.309469699859619</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1.000000000000019</v>
+      </c>
+      <c r="B46" t="n">
+        <v>-1252752377.189279</v>
+      </c>
+      <c r="C46" t="n">
+        <v>7.628774642944336</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.2177721261978149</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.417239189147949</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-8.012555122375488</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-6.015175342559814</v>
+      </c>
+      <c r="H46" t="n">
+        <v>5.042635440826416</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.9999999999999979</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1936407098.723585</v>
+      </c>
+      <c r="C47" t="n">
+        <v>7.653347969055176</v>
+      </c>
+      <c r="D47" t="n">
+        <v>-4.840800285339355</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1.896527528762817</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-8.074653625488281</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-11.17644691467285</v>
+      </c>
+      <c r="H47" t="n">
+        <v>4.456645488739014</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" t="n">
+        <v>-537007727.6064098</v>
+      </c>
+      <c r="C48" t="n">
+        <v>5.294293880462646</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-8.936630249023438</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-0.9915367364883423</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-9.520320892333984</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-13.54607009887695</v>
+      </c>
+      <c r="H48" t="n">
+        <v>4.707723617553711</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1</v>
+      </c>
+      <c r="B49" t="n">
+        <v>172694985.3418977</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1.779324531555176</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-11.2612771987915</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-0.5415372252464294</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-9.469868659973145</v>
+      </c>
+      <c r="G49" t="n">
+        <v>-7.548924446105957</v>
+      </c>
+      <c r="H49" t="n">
+        <v>4.55206298828125</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" t="n">
+        <v>140791263.8711056</v>
+      </c>
+      <c r="C50" t="n">
+        <v>5.794784069061279</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-10.01843070983887</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-2.490528345108032</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-10.76559734344482</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-6.033401966094971</v>
+      </c>
+      <c r="H50" t="n">
+        <v>6.429047107696533</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1</v>
+      </c>
+      <c r="B51" t="n">
+        <v>11656926.325853</v>
+      </c>
+      <c r="C51" t="n">
+        <v>4.51434326171875</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-7.657394886016846</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-3.969679594039917</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-9.930767059326172</v>
+      </c>
+      <c r="G51" t="n">
+        <v>-4.862458229064941</v>
+      </c>
+      <c r="H51" t="n">
+        <v>8.647357940673828</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1</v>
+      </c>
+      <c r="B52" t="n">
+        <v>11656926.325853</v>
+      </c>
+      <c r="C52" t="n">
+        <v>3.838231801986694</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-6.67451286315918</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-5.057930946350098</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-10.97615623474121</v>
+      </c>
+      <c r="G52" t="n">
+        <v>-5.308623790740967</v>
+      </c>
+      <c r="H52" t="n">
+        <v>7.221131324768066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the scaling from nn and correct urdf model
</commit_message>
<xml_diff>
--- a/exo_control/neural_network_parameters/excel/PV_cp_cnn.xlsx
+++ b/exo_control/neural_network_parameters/excel/PV_cp_cnn.xlsx
@@ -483,1322 +483,1322 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5.653803825378418</v>
+        <v>5.817864894866943</v>
       </c>
       <c r="D2" t="n">
-        <v>-9.45506477355957</v>
+        <v>-6.206963062286377</v>
       </c>
       <c r="E2" t="n">
-        <v>-4.90446662902832</v>
+        <v>-3.682085514068604</v>
       </c>
       <c r="F2" t="n">
-        <v>-9.836400032043457</v>
+        <v>-7.155896186828613</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.899656057357788</v>
+        <v>-3.445140838623047</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6799779534339905</v>
+        <v>0.7025188207626343</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.03955951504409314</v>
+        <v>0.0438359908759594</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1568202170729637</v>
+        <v>0.06737338051199913</v>
       </c>
       <c r="C3" t="n">
-        <v>6.982532501220703</v>
+        <v>4.561009407043457</v>
       </c>
       <c r="D3" t="n">
-        <v>-7.362154483795166</v>
+        <v>-6.230875492095947</v>
       </c>
       <c r="E3" t="n">
-        <v>-5.915628433227539</v>
+        <v>-3.564561128616333</v>
       </c>
       <c r="F3" t="n">
-        <v>-10.17363929748535</v>
+        <v>-7.654288768768311</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1271894425153732</v>
+        <v>0.267302542924881</v>
       </c>
       <c r="H3" t="n">
-        <v>-3.742504596710205</v>
+        <v>-4.871716499328613</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.0760839606821537</v>
+        <v>0.04572806999087334</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7650198936462402</v>
+        <v>0.2909671700000763</v>
       </c>
       <c r="C4" t="n">
-        <v>3.098288774490356</v>
+        <v>4.506760120391846</v>
       </c>
       <c r="D4" t="n">
-        <v>-7.170287609100342</v>
+        <v>-7.190632343292236</v>
       </c>
       <c r="E4" t="n">
-        <v>-5.422814846038818</v>
+        <v>-2.212725400924683</v>
       </c>
       <c r="F4" t="n">
-        <v>-8.191237449645996</v>
+        <v>-9.308317184448242</v>
       </c>
       <c r="G4" t="n">
-        <v>3.839830875396729</v>
+        <v>1.992379784584045</v>
       </c>
       <c r="H4" t="n">
-        <v>-8.351227760314941</v>
+        <v>-8.082217216491699</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.07078120946884156</v>
+        <v>0.1457655772566795</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.576290118694305</v>
+        <v>-0.1463352954387665</v>
       </c>
       <c r="C5" t="n">
-        <v>3.276397943496704</v>
+        <v>1.638507127761841</v>
       </c>
       <c r="D5" t="n">
-        <v>-4.016393184661865</v>
+        <v>-5.299228668212891</v>
       </c>
       <c r="E5" t="n">
-        <v>-5.721666812896729</v>
+        <v>-1.662243604660034</v>
       </c>
       <c r="F5" t="n">
-        <v>-6.446614265441895</v>
+        <v>-6.073385238647461</v>
       </c>
       <c r="G5" t="n">
-        <v>6.625461578369141</v>
+        <v>6.408739566802979</v>
       </c>
       <c r="H5" t="n">
-        <v>-8.255023956298828</v>
+        <v>-9.264137268066406</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.149731317460537</v>
+        <v>0.2000405177474022</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.888343858718872</v>
+        <v>-0.07551197588443756</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6246141791343689</v>
+        <v>0.08234861493110657</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.865157127380371</v>
+        <v>-4.81975269317627</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.726386070251465</v>
+        <v>-2.896986484527588</v>
       </c>
       <c r="F6" t="n">
-        <v>-5.775547981262207</v>
+        <v>-6.597298622131348</v>
       </c>
       <c r="G6" t="n">
-        <v>12.28879928588867</v>
+        <v>6.862775802612305</v>
       </c>
       <c r="H6" t="n">
-        <v>-9.456803321838379</v>
+        <v>-9.167514801025391</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1488613161444664</v>
+        <v>0.183628340959549</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.7408175563812256</v>
+        <v>-0.308225639462471</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6538363099098206</v>
+        <v>0.5529151558876038</v>
       </c>
       <c r="D7" t="n">
-        <v>-7.128524303436279</v>
+        <v>-6.099396228790283</v>
       </c>
       <c r="E7" t="n">
-        <v>-5.34001350402832</v>
+        <v>-1.86122190952301</v>
       </c>
       <c r="F7" t="n">
-        <v>-8.243284225463867</v>
+        <v>-4.875806331634521</v>
       </c>
       <c r="G7" t="n">
-        <v>11.89204502105713</v>
+        <v>9.38731861114502</v>
       </c>
       <c r="H7" t="n">
-        <v>-10.34447765350342</v>
+        <v>-9.737720489501953</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.08749550953507423</v>
+        <v>0.1580363708734512</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.7135080575943</v>
+        <v>-0.5592537784576417</v>
       </c>
       <c r="C8" t="n">
-        <v>2.714996576309204</v>
+        <v>1.28668212890625</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.651477813720703</v>
+        <v>-1.802119612693787</v>
       </c>
       <c r="E8" t="n">
-        <v>-3.041460037231445</v>
+        <v>1.095797300338745</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.850562691688538</v>
+        <v>-3.018833160400391</v>
       </c>
       <c r="G8" t="n">
-        <v>10.56995105743408</v>
+        <v>9.127470016479492</v>
       </c>
       <c r="H8" t="n">
-        <v>-11.51589393615723</v>
+        <v>-6.694605827331543</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1338613751530647</v>
+        <v>0.2464284256100655</v>
       </c>
       <c r="B9" t="n">
-        <v>-4.032371563911438</v>
+        <v>-0.2798381346464157</v>
       </c>
       <c r="C9" t="n">
-        <v>1.157655715942383</v>
+        <v>-1.247674822807312</v>
       </c>
       <c r="D9" t="n">
-        <v>-8.476902008056641</v>
+        <v>-5.999468326568604</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.8703367710113525</v>
+        <v>1.376518964767456</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.164852261543274</v>
+        <v>-5.08580207824707</v>
       </c>
       <c r="G9" t="n">
-        <v>17.68305778503418</v>
+        <v>10.96492481231689</v>
       </c>
       <c r="H9" t="n">
-        <v>-6.705341815948486</v>
+        <v>-5.830181121826172</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2425306838750839</v>
+        <v>0.3075183290243149</v>
       </c>
       <c r="B10" t="n">
-        <v>-4.553830766677857</v>
+        <v>-0.8005529081821442</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.492339611053467</v>
+        <v>-2.999230623245239</v>
       </c>
       <c r="D10" t="n">
-        <v>-6.409841060638428</v>
+        <v>-4.23090934753418</v>
       </c>
       <c r="E10" t="n">
-        <v>1.015111923217773</v>
+        <v>1.805667400360107</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.04346291720867157</v>
+        <v>-1.233830094337463</v>
       </c>
       <c r="G10" t="n">
-        <v>13.41067504882812</v>
+        <v>6.96634578704834</v>
       </c>
       <c r="H10" t="n">
-        <v>-4.840447425842285</v>
+        <v>-2.493878841400146</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.244720171391964</v>
+        <v>0.2418790990114212</v>
       </c>
       <c r="B11" t="n">
-        <v>-4.495678539276123</v>
+        <v>-1.100981800556183</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.565879583358765</v>
+        <v>-1.117237687110901</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.289535999298096</v>
+        <v>-5.862997055053711</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3835521340370178</v>
+        <v>1.393701195716858</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.1685182899236679</v>
+        <v>0.988584041595459</v>
       </c>
       <c r="G11" t="n">
-        <v>16.39345359802246</v>
+        <v>6.350520133972168</v>
       </c>
       <c r="H11" t="n">
-        <v>-1.915578365325928</v>
+        <v>-1.911917448043823</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.3026859045028686</v>
+        <v>0.292215940952301</v>
       </c>
       <c r="B12" t="n">
-        <v>-6.227140626907349</v>
+        <v>-1.189889743328095</v>
       </c>
       <c r="C12" t="n">
-        <v>-4.512838363647461</v>
+        <v>-2.560484409332275</v>
       </c>
       <c r="D12" t="n">
-        <v>-6.855685710906982</v>
+        <v>-8.30005931854248</v>
       </c>
       <c r="E12" t="n">
-        <v>2.22714900970459</v>
+        <v>2.155624628067017</v>
       </c>
       <c r="F12" t="n">
-        <v>3.554962158203125</v>
+        <v>1.646277189254761</v>
       </c>
       <c r="G12" t="n">
-        <v>16.55867767333984</v>
+        <v>6.047392845153809</v>
       </c>
       <c r="H12" t="n">
-        <v>-2.643069744110107</v>
+        <v>1.120213508605957</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.2357800707221031</v>
+        <v>0.2816279554367065</v>
       </c>
       <c r="B13" t="n">
-        <v>-7.360333452224732</v>
+        <v>-0.7176841139793396</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.265599489212036</v>
+        <v>-2.256908178329468</v>
       </c>
       <c r="D13" t="n">
-        <v>-2.806259632110596</v>
+        <v>-3.155268430709839</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1785293221473694</v>
+        <v>1.640745043754578</v>
       </c>
       <c r="F13" t="n">
-        <v>5.991874694824219</v>
+        <v>-1.846849679946899</v>
       </c>
       <c r="G13" t="n">
-        <v>15.9516134262085</v>
+        <v>7.034878730773926</v>
       </c>
       <c r="H13" t="n">
-        <v>1.183537840843201</v>
+        <v>1.689127445220947</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.3643946492671967</v>
+        <v>0.2415931895375252</v>
       </c>
       <c r="B14" t="n">
-        <v>-7.376822662353516</v>
+        <v>-1.268831021785736</v>
       </c>
       <c r="C14" t="n">
-        <v>-6.585517406463623</v>
+        <v>-1.109039783477783</v>
       </c>
       <c r="D14" t="n">
-        <v>-5.782844543457031</v>
+        <v>-2.889808654785156</v>
       </c>
       <c r="E14" t="n">
-        <v>3.989960670471191</v>
+        <v>3.603673696517944</v>
       </c>
       <c r="F14" t="n">
-        <v>6.027334213256836</v>
+        <v>2.230242729187012</v>
       </c>
       <c r="G14" t="n">
-        <v>12.59235954284668</v>
+        <v>3.108963489532471</v>
       </c>
       <c r="H14" t="n">
-        <v>0.04213961586356163</v>
+        <v>2.75834584236145</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.3006063675880432</v>
+        <v>0.2881400448083878</v>
       </c>
       <c r="B15" t="n">
-        <v>-7.597548503875733</v>
+        <v>-1.506545960903168</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.442989826202393</v>
+        <v>-2.443620920181274</v>
       </c>
       <c r="D15" t="n">
-        <v>-4.515466213226318</v>
+        <v>-4.539594173431396</v>
       </c>
       <c r="E15" t="n">
-        <v>4.235147476196289</v>
+        <v>5.050358295440674</v>
       </c>
       <c r="F15" t="n">
-        <v>6.502001285552979</v>
+        <v>3.988731861114502</v>
       </c>
       <c r="G15" t="n">
-        <v>12.2869758605957</v>
+        <v>1.448248267173767</v>
       </c>
       <c r="H15" t="n">
-        <v>0.773665726184845</v>
+        <v>4.896442890167236</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.3208064460754395</v>
+        <v>0.3604263502359391</v>
       </c>
       <c r="B16" t="n">
-        <v>-6.547559900283813</v>
+        <v>-1.407917506694794</v>
       </c>
       <c r="C16" t="n">
-        <v>-5.121472358703613</v>
+        <v>-4.51619815826416</v>
       </c>
       <c r="D16" t="n">
-        <v>-7.078282833099365</v>
+        <v>-4.848105430603027</v>
       </c>
       <c r="E16" t="n">
-        <v>5.727447509765625</v>
+        <v>5.22115421295166</v>
       </c>
       <c r="F16" t="n">
-        <v>4.2440185546875</v>
+        <v>3.25913143157959</v>
       </c>
       <c r="G16" t="n">
-        <v>6.770132541656494</v>
+        <v>-1.685045003890991</v>
       </c>
       <c r="H16" t="n">
-        <v>2.436364650726318</v>
+        <v>3.541904926300049</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.3284795796871186</v>
+        <v>0.3331609386205673</v>
       </c>
       <c r="B17" t="n">
-        <v>-7.392401561737061</v>
+        <v>-1.59396359205246</v>
       </c>
       <c r="C17" t="n">
-        <v>-5.379199504852295</v>
+        <v>-3.734450101852417</v>
       </c>
       <c r="D17" t="n">
-        <v>-4.869113445281982</v>
+        <v>-5.531632900238037</v>
       </c>
       <c r="E17" t="n">
-        <v>5.340146541595459</v>
+        <v>5.223424911499023</v>
       </c>
       <c r="F17" t="n">
-        <v>6.060836791992188</v>
+        <v>4.635401248931885</v>
       </c>
       <c r="G17" t="n">
-        <v>5.522574424743652</v>
+        <v>-4.69126558303833</v>
       </c>
       <c r="H17" t="n">
-        <v>0.8118055462837219</v>
+        <v>1.654084205627441</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.3895710784196854</v>
+        <v>0.2782755124568939</v>
       </c>
       <c r="B18" t="n">
-        <v>-7.376628570556641</v>
+        <v>-1.33558242559433</v>
       </c>
       <c r="C18" t="n">
-        <v>-7.431145191192627</v>
+        <v>-2.160786867141724</v>
       </c>
       <c r="D18" t="n">
-        <v>-4.544234275817871</v>
+        <v>-8.258331298828125</v>
       </c>
       <c r="E18" t="n">
-        <v>5.811061382293701</v>
+        <v>5.448645114898682</v>
       </c>
       <c r="F18" t="n">
-        <v>6.026916980743408</v>
+        <v>2.724034309387207</v>
       </c>
       <c r="G18" t="n">
-        <v>1.159028649330139</v>
+        <v>-4.8515305519104</v>
       </c>
       <c r="H18" t="n">
-        <v>2.008039474487305</v>
+        <v>1.639225602149963</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.345938048362732</v>
+        <v>0.4188265943527222</v>
       </c>
       <c r="B19" t="n">
-        <v>-7.189318361282349</v>
+        <v>-1.135362458229065</v>
       </c>
       <c r="C19" t="n">
-        <v>-5.965595245361328</v>
+        <v>-6.190635681152344</v>
       </c>
       <c r="D19" t="n">
-        <v>-5.017333507537842</v>
+        <v>-1.274592280387878</v>
       </c>
       <c r="E19" t="n">
-        <v>7.390029907226562</v>
+        <v>3.542989253997803</v>
       </c>
       <c r="F19" t="n">
-        <v>5.624109745025635</v>
+        <v>1.242912769317627</v>
       </c>
       <c r="G19" t="n">
-        <v>2.51450514793396</v>
+        <v>-8.232430458068848</v>
       </c>
       <c r="H19" t="n">
-        <v>1.768268227577209</v>
+        <v>1.890231490135193</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.3840714317560196</v>
+        <v>0.3449855643510819</v>
       </c>
       <c r="B20" t="n">
-        <v>-6.799793815612794</v>
+        <v>-1.064116489887238</v>
       </c>
       <c r="C20" t="n">
-        <v>-7.24642276763916</v>
+        <v>-4.073482990264893</v>
       </c>
       <c r="D20" t="n">
-        <v>-6.374450206756592</v>
+        <v>-3.811311006546021</v>
       </c>
       <c r="E20" t="n">
-        <v>5.963458061218262</v>
+        <v>5.699129581451416</v>
       </c>
       <c r="F20" t="n">
-        <v>4.786443710327148</v>
+        <v>0.7158732414245605</v>
       </c>
       <c r="G20" t="n">
-        <v>-3.265783548355103</v>
+        <v>-6.501682281494141</v>
       </c>
       <c r="H20" t="n">
-        <v>1.997541308403015</v>
+        <v>0.419753223657608</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.2890308326482773</v>
+        <v>0.4037551009654999</v>
       </c>
       <c r="B21" t="n">
-        <v>-7.633254823684693</v>
+        <v>-0.8684749281406403</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.054190158843994</v>
+        <v>-5.758508682250977</v>
       </c>
       <c r="D21" t="n">
-        <v>-7.59557580947876</v>
+        <v>-4.309493541717529</v>
       </c>
       <c r="E21" t="n">
-        <v>7.018465995788574</v>
+        <v>3.978034019470215</v>
       </c>
       <c r="F21" t="n">
-        <v>6.578786849975586</v>
+        <v>-0.731378972530365</v>
       </c>
       <c r="G21" t="n">
-        <v>-4.501266479492188</v>
+        <v>-11.51800155639648</v>
       </c>
       <c r="H21" t="n">
-        <v>2.374178409576416</v>
+        <v>-0.5955670475959778</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.3386340808868408</v>
+        <v>0.3952068167924881</v>
       </c>
       <c r="B22" t="n">
-        <v>-6.609446372985841</v>
+        <v>-0.92730508685112</v>
       </c>
       <c r="C22" t="n">
-        <v>-5.720269203186035</v>
+        <v>-5.513414859771729</v>
       </c>
       <c r="D22" t="n">
-        <v>-3.579771995544434</v>
+        <v>-3.469545364379883</v>
       </c>
       <c r="E22" t="n">
-        <v>7.549747943878174</v>
+        <v>3.262240648269653</v>
       </c>
       <c r="F22" t="n">
-        <v>4.377104759216309</v>
+        <v>-0.296184778213501</v>
       </c>
       <c r="G22" t="n">
-        <v>-10.92592334747314</v>
+        <v>-11.06823062896729</v>
       </c>
       <c r="H22" t="n">
-        <v>1.854192852973938</v>
+        <v>-2.132184743881226</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.4411210888624191</v>
+        <v>0.3855885636806488</v>
       </c>
       <c r="B23" t="n">
-        <v>-5.940849161148072</v>
+        <v>-1.144380776882172</v>
       </c>
       <c r="C23" t="n">
-        <v>-9.162611961364746</v>
+        <v>-5.237642288208008</v>
       </c>
       <c r="D23" t="n">
-        <v>-4.251810073852539</v>
+        <v>-3.787387371063232</v>
       </c>
       <c r="E23" t="n">
-        <v>6.078746795654297</v>
+        <v>3.289721965789795</v>
       </c>
       <c r="F23" t="n">
-        <v>2.939297437667847</v>
+        <v>1.309626340866089</v>
       </c>
       <c r="G23" t="n">
-        <v>-9.47633171081543</v>
+        <v>-8.671011924743652</v>
       </c>
       <c r="H23" t="n">
-        <v>0.6368582844734192</v>
+        <v>-2.808276653289795</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.4456500554084778</v>
+        <v>0.3889022767543793</v>
       </c>
       <c r="B24" t="n">
-        <v>-6.180853271484375</v>
+        <v>-1.169432265758515</v>
       </c>
       <c r="C24" t="n">
-        <v>-9.314731597900391</v>
+        <v>-5.332652568817139</v>
       </c>
       <c r="D24" t="n">
-        <v>-4.079325199127197</v>
+        <v>-1.316652059555054</v>
       </c>
       <c r="E24" t="n">
-        <v>4.485651016235352</v>
+        <v>2.758493423461914</v>
       </c>
       <c r="F24" t="n">
-        <v>3.455422878265381</v>
+        <v>1.494943857192993</v>
       </c>
       <c r="G24" t="n">
-        <v>-9.130809783935547</v>
+        <v>-11.60657691955566</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1205405294895172</v>
+        <v>-2.027732372283936</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.491607638001442</v>
+        <v>0.383024492263794</v>
       </c>
       <c r="B25" t="n">
-        <v>-6.48880467414856</v>
+        <v>-1.240144608020783</v>
       </c>
       <c r="C25" t="n">
-        <v>-10.85835933685303</v>
+        <v>-5.164126396179199</v>
       </c>
       <c r="D25" t="n">
-        <v>-4.731420993804932</v>
+        <v>-3.737834930419922</v>
       </c>
       <c r="E25" t="n">
-        <v>3.573874473571777</v>
+        <v>2.087876319885254</v>
       </c>
       <c r="F25" t="n">
-        <v>4.117667198181152</v>
+        <v>2.018035650253296</v>
       </c>
       <c r="G25" t="n">
-        <v>-11.33881282806396</v>
+        <v>-8.304347991943359</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.8750782012939453</v>
+        <v>-2.728530883789062</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.4214950090646744</v>
+        <v>0.5030275583267212</v>
       </c>
       <c r="B26" t="n">
-        <v>-6.662927255630493</v>
+        <v>-1.692302045822144</v>
       </c>
       <c r="C26" t="n">
-        <v>-8.503409385681152</v>
+        <v>-8.604825973510742</v>
       </c>
       <c r="D26" t="n">
-        <v>-2.92297625541687</v>
+        <v>-3.713050842285156</v>
       </c>
       <c r="E26" t="n">
-        <v>4.289812564849854</v>
+        <v>0.5730848908424377</v>
       </c>
       <c r="F26" t="n">
-        <v>4.492114067077637</v>
+        <v>5.362856864929199</v>
       </c>
       <c r="G26" t="n">
-        <v>-11.95578861236572</v>
+        <v>-4.106042861938477</v>
       </c>
       <c r="H26" t="n">
-        <v>0.03409799560904503</v>
+        <v>-2.788376569747925</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.53</v>
+        <v>0.5256192243099213</v>
       </c>
       <c r="B27" t="n">
-        <v>-6.60126368522644</v>
+        <v>-1.908880438804627</v>
       </c>
       <c r="C27" t="n">
-        <v>-12.14788627624512</v>
+        <v>-9.252570152282715</v>
       </c>
       <c r="D27" t="n">
-        <v>-2.128310680389404</v>
+        <v>-0.8258281350135803</v>
       </c>
       <c r="E27" t="n">
-        <v>2.17871880531311</v>
+        <v>-1.706596255302429</v>
       </c>
       <c r="F27" t="n">
-        <v>4.359508037567139</v>
+        <v>6.964989185333252</v>
       </c>
       <c r="G27" t="n">
-        <v>-11.91915321350098</v>
+        <v>-4.341679096221924</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.1532654166221619</v>
+        <v>-2.569894790649414</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.4611238217353821</v>
+        <v>0.440703210234642</v>
       </c>
       <c r="B28" t="n">
-        <v>-7.341657676696777</v>
+        <v>-2.271510634422302</v>
       </c>
       <c r="C28" t="n">
-        <v>-9.834465980529785</v>
+        <v>-6.817877292633057</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4804942607879639</v>
+        <v>0.8665604591369629</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.681118369102478</v>
+        <v>-2.266187191009521</v>
       </c>
       <c r="F28" t="n">
-        <v>5.951713085174561</v>
+        <v>9.64753532409668</v>
       </c>
       <c r="G28" t="n">
-        <v>-9.12940788269043</v>
+        <v>-1.564961194992065</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.706722617149353</v>
+        <v>-2.124371767044067</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.3765462678670883</v>
+        <v>0.5126251196861268</v>
       </c>
       <c r="B29" t="n">
-        <v>-6.523819541931153</v>
+        <v>-2.133577075004578</v>
       </c>
       <c r="C29" t="n">
-        <v>-6.993666648864746</v>
+        <v>-8.8800048828125</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.3383738994598389</v>
+        <v>-0.03855109214782715</v>
       </c>
       <c r="E29" t="n">
-        <v>-2.455382108688354</v>
+        <v>-6.027772426605225</v>
       </c>
       <c r="F29" t="n">
-        <v>4.192965507507324</v>
+        <v>8.627175331115723</v>
       </c>
       <c r="G29" t="n">
-        <v>-6.344018459320068</v>
+        <v>0.9376700520515442</v>
       </c>
       <c r="H29" t="n">
-        <v>-5.332154750823975</v>
+        <v>-3.249444961547852</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.3696409088373184</v>
+        <v>0.5004397940635681</v>
       </c>
       <c r="B30" t="n">
-        <v>-7.121702642440797</v>
+        <v>-2.239950752258301</v>
       </c>
       <c r="C30" t="n">
-        <v>-6.76172924041748</v>
+        <v>-8.530631065368652</v>
       </c>
       <c r="D30" t="n">
-        <v>3.226950407028198</v>
+        <v>2.387399435043335</v>
       </c>
       <c r="E30" t="n">
-        <v>-7.505757331848145</v>
+        <v>-8.489104270935059</v>
       </c>
       <c r="F30" t="n">
-        <v>5.478703498840332</v>
+        <v>9.414073944091797</v>
       </c>
       <c r="G30" t="n">
-        <v>-7.42233943939209</v>
+        <v>2.185237169265747</v>
       </c>
       <c r="H30" t="n">
-        <v>-2.978699445724487</v>
+        <v>-3.461441040039062</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.2783848470449448</v>
+        <v>0.53</v>
       </c>
       <c r="B31" t="n">
-        <v>-5.707650899887085</v>
+        <v>-2.207491173744202</v>
       </c>
       <c r="C31" t="n">
-        <v>-3.696612119674683</v>
+        <v>-9.378174781799316</v>
       </c>
       <c r="D31" t="n">
-        <v>1.489211082458496</v>
+        <v>-0.7991624474525452</v>
       </c>
       <c r="E31" t="n">
-        <v>-8.876958847045898</v>
+        <v>-12.69013214111328</v>
       </c>
       <c r="F31" t="n">
-        <v>2.437807559967041</v>
+        <v>9.173953056335449</v>
       </c>
       <c r="G31" t="n">
-        <v>-3.759764671325684</v>
+        <v>2.578437089920044</v>
       </c>
       <c r="H31" t="n">
-        <v>-3.03329873085022</v>
+        <v>-1.796664714813232</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.3707437318563461</v>
+        <v>0.5147156816720962</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.77438497543335</v>
+        <v>-2.253185133934021</v>
       </c>
       <c r="C32" t="n">
-        <v>-6.798770904541016</v>
+        <v>-8.939945220947266</v>
       </c>
       <c r="D32" t="n">
-        <v>6.546842098236084</v>
+        <v>0.6072109937667847</v>
       </c>
       <c r="E32" t="n">
-        <v>-11.294677734375</v>
+        <v>-15.00915336608887</v>
       </c>
       <c r="F32" t="n">
-        <v>4.731802463531494</v>
+        <v>9.511972427368164</v>
       </c>
       <c r="G32" t="n">
-        <v>-2.677718639373779</v>
+        <v>5.976258277893066</v>
       </c>
       <c r="H32" t="n">
-        <v>-4.939930438995361</v>
+        <v>-0.7118256092071533</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.2245207720994949</v>
+        <v>0.4427243995666504</v>
       </c>
       <c r="B33" t="n">
-        <v>-6.712632446289063</v>
+        <v>-1.899984059333801</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.887420892715454</v>
+        <v>-6.875827789306641</v>
       </c>
       <c r="D33" t="n">
-        <v>6.690071105957031</v>
+        <v>3.504192590713501</v>
       </c>
       <c r="E33" t="n">
-        <v>-11.49570274353027</v>
+        <v>-15.76076030731201</v>
       </c>
       <c r="F33" t="n">
-        <v>4.599004745483398</v>
+        <v>6.899178981781006</v>
       </c>
       <c r="G33" t="n">
-        <v>-5.09229040145874</v>
+        <v>4.637758255004883</v>
       </c>
       <c r="H33" t="n">
-        <v>-2.373816728591919</v>
+        <v>0.7767148017883301</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.1530321574211121</v>
+        <v>0.4521480870246887</v>
       </c>
       <c r="B34" t="n">
-        <v>-5.939880723953247</v>
+        <v>-1.726754603385925</v>
       </c>
       <c r="C34" t="n">
-        <v>0.5137457251548767</v>
+        <v>-7.146022319793701</v>
       </c>
       <c r="D34" t="n">
-        <v>9.677059173583984</v>
+        <v>4.790561676025391</v>
       </c>
       <c r="E34" t="n">
-        <v>-12.36382675170898</v>
+        <v>-13.60810852050781</v>
       </c>
       <c r="F34" t="n">
-        <v>2.937215328216553</v>
+        <v>5.617718696594238</v>
       </c>
       <c r="G34" t="n">
-        <v>-4.109493732452393</v>
+        <v>3.63223123550415</v>
       </c>
       <c r="H34" t="n">
-        <v>0.7524218559265137</v>
+        <v>0.5588850378990173</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.5760446442309581</v>
+        <v>0.6102559934456562</v>
       </c>
       <c r="B35" t="n">
-        <v>67.12821872158977</v>
+        <v>12.1155701458018</v>
       </c>
       <c r="C35" t="n">
-        <v>-3.256949663162231</v>
+        <v>-4.99265718460083</v>
       </c>
       <c r="D35" t="n">
-        <v>9.320235252380371</v>
+        <v>7.839961528778076</v>
       </c>
       <c r="E35" t="n">
-        <v>-12.42622756958008</v>
+        <v>-11.71665287017822</v>
       </c>
       <c r="F35" t="n">
-        <v>1.024024367332458</v>
+        <v>8.826605796813965</v>
       </c>
       <c r="G35" t="n">
-        <v>-2.465534210205078</v>
+        <v>8.118843078613281</v>
       </c>
       <c r="H35" t="n">
-        <v>0.166785255074501</v>
+        <v>2.944969177246094</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.9258429132933984</v>
+        <v>0.7976842349473292</v>
       </c>
       <c r="B36" t="n">
-        <v>-598.0477792531145</v>
+        <v>-31.29313860536108</v>
       </c>
       <c r="C36" t="n">
-        <v>2.539982080459595</v>
+        <v>-2.070385694503784</v>
       </c>
       <c r="D36" t="n">
-        <v>12.40510082244873</v>
+        <v>7.788970470428467</v>
       </c>
       <c r="E36" t="n">
-        <v>-7.936156749725342</v>
+        <v>-9.18409538269043</v>
       </c>
       <c r="F36" t="n">
-        <v>0.4885174036026001</v>
+        <v>4.23446798324585</v>
       </c>
       <c r="G36" t="n">
-        <v>-5.672225475311279</v>
+        <v>5.782907009124756</v>
       </c>
       <c r="H36" t="n">
-        <v>-1.611362099647522</v>
+        <v>2.701654195785522</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.9854273361874343</v>
+        <v>0.9083198700254053</v>
       </c>
       <c r="B37" t="n">
-        <v>6025.956393897622</v>
+        <v>87.89986730496067</v>
       </c>
       <c r="C37" t="n">
-        <v>2.155580759048462</v>
+        <v>-1.068275928497314</v>
       </c>
       <c r="D37" t="n">
-        <v>12.78581237792969</v>
+        <v>11.6503791809082</v>
       </c>
       <c r="E37" t="n">
-        <v>-5.631823539733887</v>
+        <v>-5.08844518661499</v>
       </c>
       <c r="F37" t="n">
-        <v>1.626761674880981</v>
+        <v>3.394479751586914</v>
       </c>
       <c r="G37" t="n">
-        <v>-3.977789640426636</v>
+        <v>2.56387734413147</v>
       </c>
       <c r="H37" t="n">
-        <v>0.4700658321380615</v>
+        <v>3.225723266601562</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.9994786432932744</v>
+        <v>0.9730676950777303</v>
       </c>
       <c r="B38" t="n">
-        <v>-49178.69888090814</v>
+        <v>-217.8481627842617</v>
       </c>
       <c r="C38" t="n">
-        <v>5.016924381256104</v>
+        <v>1.353818416595459</v>
       </c>
       <c r="D38" t="n">
-        <v>12.49951267242432</v>
+        <v>13.25100421905518</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.9030991792678833</v>
+        <v>-0.6803759336471558</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.5329524874687195</v>
+        <v>2.717870950698853</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.772716522216797</v>
+        <v>2.385239601135254</v>
       </c>
       <c r="H38" t="n">
-        <v>1.688389897346497</v>
+        <v>5.642911434173584</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.9999257146760382</v>
+        <v>0.9925197967229298</v>
       </c>
       <c r="B39" t="n">
-        <v>433650.9197279753</v>
+        <v>313.5500096013426</v>
       </c>
       <c r="C39" t="n">
-        <v>3.117336511611938</v>
+        <v>1.597303152084351</v>
       </c>
       <c r="D39" t="n">
-        <v>11.91916275024414</v>
+        <v>8.603158950805664</v>
       </c>
       <c r="E39" t="n">
-        <v>2.331615924835205</v>
+        <v>0.6442989110946655</v>
       </c>
       <c r="F39" t="n">
-        <v>0.2135843187570572</v>
+        <v>-1.556571006774902</v>
       </c>
       <c r="G39" t="n">
-        <v>-3.424475431442261</v>
+        <v>0.7967022061347961</v>
       </c>
       <c r="H39" t="n">
-        <v>1.144328236579895</v>
+        <v>2.969263792037964</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.999999749297701</v>
+        <v>0.9984764344326534</v>
       </c>
       <c r="B40" t="n">
-        <v>-3191328.746648094</v>
+        <v>-490.5854035085606</v>
       </c>
       <c r="C40" t="n">
-        <v>5.593725681304932</v>
+        <v>2.722740173339844</v>
       </c>
       <c r="D40" t="n">
-        <v>11.59312152862549</v>
+        <v>9.597941398620605</v>
       </c>
       <c r="E40" t="n">
-        <v>1.168919086456299</v>
+        <v>4.855470657348633</v>
       </c>
       <c r="F40" t="n">
-        <v>-1.448671698570251</v>
+        <v>-0.9893990159034729</v>
       </c>
       <c r="G40" t="n">
-        <v>-3.680985927581787</v>
+        <v>-0.3053227365016937</v>
       </c>
       <c r="H40" t="n">
-        <v>1.698674321174622</v>
+        <v>4.27837085723877</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1.000000001762465</v>
+        <v>1.000011391075531</v>
       </c>
       <c r="B41" t="n">
-        <v>19699683.16564975</v>
+        <v>487.2853661159463</v>
       </c>
       <c r="C41" t="n">
-        <v>5.778951644897461</v>
+        <v>5.931479454040527</v>
       </c>
       <c r="D41" t="n">
-        <v>10.50806140899658</v>
+        <v>4.788771152496338</v>
       </c>
       <c r="E41" t="n">
-        <v>6.034224510192871</v>
+        <v>4.916810035705566</v>
       </c>
       <c r="F41" t="n">
-        <v>-2.800826549530029</v>
+        <v>-3.277507781982422</v>
       </c>
       <c r="G41" t="n">
-        <v>-4.035259246826172</v>
+        <v>-3.757441520690918</v>
       </c>
       <c r="H41" t="n">
-        <v>3.173066854476929</v>
+        <v>2.602213621139526</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.9999999997511972</v>
+        <v>1.000002143642736</v>
       </c>
       <c r="B42" t="n">
-        <v>-65333767.48886446</v>
+        <v>-317.9823814174187</v>
       </c>
       <c r="C42" t="n">
-        <v>8.166824340820312</v>
+        <v>2.958180665969849</v>
       </c>
       <c r="D42" t="n">
-        <v>8.219392776489258</v>
+        <v>7.228627681732178</v>
       </c>
       <c r="E42" t="n">
-        <v>5.934537410736084</v>
+        <v>5.773301601409912</v>
       </c>
       <c r="F42" t="n">
-        <v>-6.056411743164062</v>
+        <v>-4.58411169052124</v>
       </c>
       <c r="G42" t="n">
-        <v>-9.089858055114746</v>
+        <v>-3.837938547134399</v>
       </c>
       <c r="H42" t="n">
-        <v>3.366066932678223</v>
+        <v>3.110602378845215</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.9999999999789329</v>
+        <v>0.9999997110043932</v>
       </c>
       <c r="B43" t="n">
-        <v>327212862.8340886</v>
+        <v>118.5467404163745</v>
       </c>
       <c r="C43" t="n">
-        <v>4.14646053314209</v>
+        <v>7.866521835327148</v>
       </c>
       <c r="D43" t="n">
-        <v>5.195571422576904</v>
+        <v>-0.4457595348358154</v>
       </c>
       <c r="E43" t="n">
-        <v>3.621502876281738</v>
+        <v>6.998164653778076</v>
       </c>
       <c r="F43" t="n">
-        <v>-4.128128528594971</v>
+        <v>-5.711112022399902</v>
       </c>
       <c r="G43" t="n">
-        <v>-5.493937492370605</v>
+        <v>-6.784659385681152</v>
       </c>
       <c r="H43" t="n">
-        <v>2.301235914230347</v>
+        <v>3.617861032485962</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1.000000000001789</v>
+        <v>1.000000012092927</v>
       </c>
       <c r="B44" t="n">
-        <v>-629447671.9172032</v>
+        <v>8.162469680999131</v>
       </c>
       <c r="C44" t="n">
-        <v>7.165080070495605</v>
+        <v>6.453738212585449</v>
       </c>
       <c r="D44" t="n">
-        <v>2.994858026504517</v>
+        <v>-1.87214457988739</v>
       </c>
       <c r="E44" t="n">
-        <v>3.516398429870605</v>
+        <v>7.105005741119385</v>
       </c>
       <c r="F44" t="n">
-        <v>-7.64389181137085</v>
+        <v>-7.394793510437012</v>
       </c>
       <c r="G44" t="n">
-        <v>-8.68282413482666</v>
+        <v>-10.29104804992676</v>
       </c>
       <c r="H44" t="n">
-        <v>3.219171047210693</v>
+        <v>1.984947800636292</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.9999999999998302</v>
+        <v>0.9999999989651992</v>
       </c>
       <c r="B45" t="n">
-        <v>782869358.9793085</v>
+        <v>3.79577875070285</v>
       </c>
       <c r="C45" t="n">
-        <v>7.343530654907227</v>
+        <v>7.11820125579834</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.4419060945510864</v>
+        <v>-5.784624576568604</v>
       </c>
       <c r="E45" t="n">
-        <v>4.416713237762451</v>
+        <v>5.993652820587158</v>
       </c>
       <c r="F45" t="n">
-        <v>-8.418839454650879</v>
+        <v>-8.686275482177734</v>
       </c>
       <c r="G45" t="n">
-        <v>-9.380785942077637</v>
+        <v>-8.96271800994873</v>
       </c>
       <c r="H45" t="n">
-        <v>4.309469699859619</v>
+        <v>2.963507175445557</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1.000000000000019</v>
+        <v>1.00000000013053</v>
       </c>
       <c r="B46" t="n">
-        <v>-1252752377.189279</v>
+        <v>0.4221643729989389</v>
       </c>
       <c r="C46" t="n">
-        <v>7.628774642944336</v>
+        <v>7.734702110290527</v>
       </c>
       <c r="D46" t="n">
-        <v>0.2177721261978149</v>
+        <v>-8.662552833557129</v>
       </c>
       <c r="E46" t="n">
-        <v>3.417239189147949</v>
+        <v>6.26251745223999</v>
       </c>
       <c r="F46" t="n">
-        <v>-8.012555122375488</v>
+        <v>-6.345568656921387</v>
       </c>
       <c r="G46" t="n">
-        <v>-6.015175342559814</v>
+        <v>-7.141335964202881</v>
       </c>
       <c r="H46" t="n">
-        <v>5.042635440826416</v>
+        <v>2.256171941757202</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.9999999999999979</v>
+        <v>0.9999999999769131</v>
       </c>
       <c r="B47" t="n">
-        <v>1936407098.723585</v>
+        <v>0.6493861998332386</v>
       </c>
       <c r="C47" t="n">
-        <v>7.653347969055176</v>
+        <v>8.505586624145508</v>
       </c>
       <c r="D47" t="n">
-        <v>-4.840800285339355</v>
+        <v>-12.26727962493896</v>
       </c>
       <c r="E47" t="n">
-        <v>1.896527528762817</v>
+        <v>1.857871770858765</v>
       </c>
       <c r="F47" t="n">
-        <v>-8.074653625488281</v>
+        <v>-9.53483772277832</v>
       </c>
       <c r="G47" t="n">
-        <v>-11.17644691467285</v>
+        <v>-8.310917854309082</v>
       </c>
       <c r="H47" t="n">
-        <v>4.456645488739014</v>
+        <v>4.185006141662598</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1</v>
+        <v>1.000000000001579</v>
       </c>
       <c r="B48" t="n">
-        <v>-537007727.6064098</v>
+        <v>0.8643610870970773</v>
       </c>
       <c r="C48" t="n">
-        <v>5.294293880462646</v>
+        <v>6.857312202453613</v>
       </c>
       <c r="D48" t="n">
-        <v>-8.936630249023438</v>
+        <v>-13.49612236022949</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.9915367364883423</v>
+        <v>0.985001802444458</v>
       </c>
       <c r="F48" t="n">
-        <v>-9.520320892333984</v>
+        <v>-8.672647476196289</v>
       </c>
       <c r="G48" t="n">
-        <v>-13.54607009887695</v>
+        <v>-7.972617626190186</v>
       </c>
       <c r="H48" t="n">
-        <v>4.707723617553711</v>
+        <v>5.392895698547363</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>1.000000000000076</v>
       </c>
       <c r="B49" t="n">
-        <v>172694985.3418977</v>
+        <v>0.8643610870970773</v>
       </c>
       <c r="C49" t="n">
-        <v>1.779324531555176</v>
+        <v>5.084320068359375</v>
       </c>
       <c r="D49" t="n">
-        <v>-11.2612771987915</v>
+        <v>-11.88940048217773</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.5415372252464294</v>
+        <v>0.2883090674877167</v>
       </c>
       <c r="F49" t="n">
-        <v>-9.469868659973145</v>
+        <v>-11.0765552520752</v>
       </c>
       <c r="G49" t="n">
-        <v>-7.548924446105957</v>
+        <v>-7.286895275115967</v>
       </c>
       <c r="H49" t="n">
-        <v>4.55206298828125</v>
+        <v>3.181580543518066</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>1.000000000000016</v>
       </c>
       <c r="B50" t="n">
-        <v>140791263.8711056</v>
+        <v>0.9142142419965084</v>
       </c>
       <c r="C50" t="n">
-        <v>5.794784069061279</v>
+        <v>2.707840442657471</v>
       </c>
       <c r="D50" t="n">
-        <v>-10.01843070983887</v>
+        <v>-12.35038757324219</v>
       </c>
       <c r="E50" t="n">
-        <v>-2.490528345108032</v>
+        <v>-1.897008299827576</v>
       </c>
       <c r="F50" t="n">
-        <v>-10.76559734344482</v>
+        <v>-9.635543823242188</v>
       </c>
       <c r="G50" t="n">
-        <v>-6.033401966094971</v>
+        <v>-8.762391090393066</v>
       </c>
       <c r="H50" t="n">
-        <v>6.429047107696533</v>
+        <v>7.889337539672852</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1</v>
+        <v>1.000000000000006</v>
       </c>
       <c r="B51" t="n">
-        <v>11656926.325853</v>
+        <v>0.9304326622869564</v>
       </c>
       <c r="C51" t="n">
-        <v>4.51434326171875</v>
+        <v>0.03581156954169273</v>
       </c>
       <c r="D51" t="n">
-        <v>-7.657394886016846</v>
+        <v>-11.98019218444824</v>
       </c>
       <c r="E51" t="n">
-        <v>-3.969679594039917</v>
+        <v>-3.574863195419312</v>
       </c>
       <c r="F51" t="n">
-        <v>-9.930767059326172</v>
+        <v>-10.33532619476318</v>
       </c>
       <c r="G51" t="n">
-        <v>-4.862458229064941</v>
+        <v>-5.041069984436035</v>
       </c>
       <c r="H51" t="n">
-        <v>8.647357940673828</v>
+        <v>6.861157894134521</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>1.000000000000002</v>
       </c>
       <c r="B52" t="n">
-        <v>11656926.325853</v>
+        <v>0.9373637612332291</v>
       </c>
       <c r="C52" t="n">
-        <v>3.838231801986694</v>
+        <v>-0.4439275562763214</v>
       </c>
       <c r="D52" t="n">
-        <v>-6.67451286315918</v>
+        <v>-8.254817008972168</v>
       </c>
       <c r="E52" t="n">
-        <v>-5.057930946350098</v>
+        <v>-4.122600555419922</v>
       </c>
       <c r="F52" t="n">
-        <v>-10.97615623474121</v>
+        <v>-10.68593406677246</v>
       </c>
       <c r="G52" t="n">
-        <v>-5.308623790740967</v>
+        <v>-1.86876392364502</v>
       </c>
       <c r="H52" t="n">
-        <v>7.221131324768066</v>
+        <v>2.797060012817383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>